<commit_message>
[FEAT] add functions (and correct typo in gram)
</commit_message>
<xml_diff>
--- a/LL1.xlsx
+++ b/LL1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theot\Documents\TELECOM\2A\Projet_compil\pcl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{155EE861-560F-485E-838C-01C9B7F63663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B78C177-9876-4AC0-B5EE-9DF155B2D52B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{6D8C16DF-770F-44B3-88DF-F08FBFD5ADCC}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13056" activeTab="1" xr2:uid="{6D8C16DF-770F-44B3-88DF-F08FBFD5ADCC}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -2547,8 +2547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D1E37C5-8300-43F0-8EE7-C57C19613C2D}">
   <dimension ref="A1:C70"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3340,8 +3340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F681F8A-924D-4ED2-9279-7655A3BABCEB}">
   <dimension ref="A1:BB70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH31" workbookViewId="0">
-      <selection activeCell="AI39" sqref="AI39"/>
+    <sheetView tabSelected="1" topLeftCell="AC49" workbookViewId="0">
+      <selection activeCell="AE55" sqref="AE55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3377,10 +3377,9 @@
     <col min="47" max="47" width="35.21875" bestFit="1" customWidth="1"/>
     <col min="48" max="49" width="32" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="32" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="82.88671875" bestFit="1" customWidth="1"/>
-    <col min="53" max="54" width="35.21875" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="82.88671875" bestFit="1" customWidth="1"/>
+    <col min="52" max="53" width="35.21875" bestFit="1" customWidth="1"/>
+    <col min="54" max="55" width="23.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:54" x14ac:dyDescent="0.3">

</xml_diff>